<commit_message>
Added store_count,address and phoneumber verification tests
</commit_message>
<xml_diff>
--- a/src/test/resources/dataFiles/llpclienttoken.xlsx
+++ b/src/test/resources/dataFiles/llpclienttoken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MF_Gitworkspace\RestAssuredpoc\restassured_poc\src\test\resources\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E580EDE-FC4F-44A2-9121-BA7E08F71B38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BCB34-BA80-4D53-B09A-5CB7C69D89DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5629D694-238F-4AC5-9D30-2A2B9B03292A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>client_name</t>
   </si>
@@ -67,6 +67,72 @@
   </si>
   <si>
     <t>RCKBBWJSPPOONTUT</t>
+  </si>
+  <si>
+    <t>WaBa Grill</t>
+  </si>
+  <si>
+    <t>store_name</t>
+  </si>
+  <si>
+    <t>Dippin' Dots</t>
+  </si>
+  <si>
+    <t>brand_name</t>
+  </si>
+  <si>
+    <t>corporate_id</t>
+  </si>
+  <si>
+    <t>Arvest Bank</t>
+  </si>
+  <si>
+    <t>Dollar Rent A Car</t>
+  </si>
+  <si>
+    <t>Cricket Wireless</t>
+  </si>
+  <si>
+    <t>Cricket Wireless Authorized Retailer</t>
+  </si>
+  <si>
+    <t>store_address</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>(402) 345-2783</t>
+  </si>
+  <si>
+    <t>(402) 885-6815</t>
+  </si>
+  <si>
+    <t>(913) 279-3300</t>
+  </si>
+  <si>
+    <t>402-393-0663</t>
+  </si>
+  <si>
+    <t>562-463-9222</t>
+  </si>
+  <si>
+    <t>13131 Crossroads Pkway S.</t>
+  </si>
+  <si>
+    <t>10000 California St.</t>
+  </si>
+  <si>
+    <t>9221 North Oak Trafficway</t>
+  </si>
+  <si>
+    <t>365 N Saddle Creek Rd</t>
+  </si>
+  <si>
+    <t>4501 ABBOT DRIVE</t>
+  </si>
+  <si>
+    <t>store_count</t>
   </si>
 </sst>
 </file>
@@ -96,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -119,14 +185,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,67 +523,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A568B9-D401-4E4D-A6AC-32DDEE00E90E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3">
+        <v>70189192</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9346132</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3">
+        <v>9002</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>964</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the framework with Enhanced Reports
</commit_message>
<xml_diff>
--- a/src/test/resources/dataFiles/llpclienttoken.xlsx
+++ b/src/test/resources/dataFiles/llpclienttoken.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MF_Gitworkspace\RestAssuredpoc\restassured_poc\src\test\resources\dataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MF_Gitworkspace\MF_1\restassured_poc\src\test\resources\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BCB34-BA80-4D53-B09A-5CB7C69D89DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0B21-16C7-4284-B053-76A7189A651D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5629D694-238F-4AC5-9D30-2A2B9B03292A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>client_name</t>
   </si>
@@ -102,50 +102,67 @@
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>(402) 345-2783</t>
-  </si>
-  <si>
-    <t>(402) 885-6815</t>
-  </si>
-  <si>
-    <t>(913) 279-3300</t>
-  </si>
-  <si>
-    <t>402-393-0663</t>
-  </si>
-  <si>
     <t>562-463-9222</t>
   </si>
   <si>
-    <t>13131 Crossroads Pkway S.</t>
-  </si>
-  <si>
-    <t>10000 California St.</t>
-  </si>
-  <si>
-    <t>9221 North Oak Trafficway</t>
-  </si>
-  <si>
-    <t>365 N Saddle Creek Rd</t>
-  </si>
-  <si>
-    <t>4501 ABBOT DRIVE</t>
-  </si>
-  <si>
     <t>store_count</t>
+  </si>
+  <si>
+    <t>80170100</t>
+  </si>
+  <si>
+    <t>800 E Dimond Blvd</t>
+  </si>
+  <si>
+    <t>3138</t>
+  </si>
+  <si>
+    <t>5725 Johnston St.</t>
+  </si>
+  <si>
+    <t>337-993-1090</t>
+  </si>
+  <si>
+    <t>68846</t>
+  </si>
+  <si>
+    <t>6470 SPALDING DR</t>
+  </si>
+  <si>
+    <t>(770) 582-0841</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5211 E. Washington Blvd.</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>3200 Rogers Ave.</t>
+  </si>
+  <si>
+    <t>(479) 709-8800</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -207,8 +224,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +545,10 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
@@ -541,7 +560,7 @@
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,10 +583,10 @@
         <v>22</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -580,20 +599,20 @@
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
-        <v>70189192</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2">
+        <v>9075220666</v>
       </c>
       <c r="H2" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -606,20 +625,20 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3">
-        <v>61</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -632,20 +651,20 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3">
-        <v>9346132</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="2">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -658,20 +677,20 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
-        <v>9002</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>28</v>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H5" s="2">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -684,17 +703,17 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3">
-        <v>964</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="H6" s="2">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>